<commit_message>
Added metric mm conversions
</commit_message>
<xml_diff>
--- a/083816_bourdon_scaling.xlsx
+++ b/083816_bourdon_scaling.xlsx
@@ -1,25 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\canti021\Documents\Project files\3D printed organ pipes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keiran\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D81F50-6507-4029-A810-E9FB23343D2C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12015"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="73">
   <si>
     <r>
       <rPr>
@@ -638,11 +647,14 @@
   <si>
     <t>Diameter</t>
   </si>
+  <si>
+    <t>Diameter_mm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;F&quot;#,##0;&quot;F&quot;\-#,##0"/>
     <numFmt numFmtId="165" formatCode="0.000."/>
@@ -734,10 +746,10 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -758,7 +770,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -797,7 +809,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1275,6 +1286,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2197-43C5-835E-22E1CA1248DE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1457,7 +1473,7 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1496,7 +1512,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1830,6 +1845,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4FAE-4714-AE77-819872ED2BB5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2012,7 +2032,7 @@
 </file>
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2026,7 +2046,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2515,6 +2534,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0B3B-4E42-B3C5-099E1D9815F5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2697,7 +2721,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2711,7 +2735,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3200,6 +3223,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EE0B-4527-99C7-7CD98C634318}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3382,7 +3410,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3396,7 +3424,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3835,6 +3862,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C73E-460A-BB1B-8ECF79E7A8E8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4017,7 +4049,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4031,7 +4063,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4520,6 +4551,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-93D0-4049-9CC3-F86EE0641D2F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4702,7 +4738,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4716,7 +4752,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4788,6 +4823,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.929195374015748E-2"/>
+                  <c:y val="-0.24385076248196291"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.0000000000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$59</c:f>
@@ -5155,6 +5240,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CADB-4C05-BE2A-54B6A150E746}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -5337,7 +5427,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5351,7 +5441,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5840,6 +5929,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0F39-4988-AF98-A805AE022EBB}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -6022,7 +6116,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6036,7 +6130,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6525,6 +6618,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1C08-46DB-A290-A17D47E9659B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -6707,7 +6805,7 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6721,7 +6819,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7210,6 +7307,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-00A5-4981-B182-2F0E1D175215}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -7392,7 +7494,7 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -7431,7 +7533,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7759,6 +7860,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4BEC-46DD-9E09-05F1CF1CAD0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -14073,7 +14179,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -14103,7 +14215,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -14133,7 +14251,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -14163,7 +14287,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -14193,7 +14323,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -14223,7 +14359,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -14253,7 +14395,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvPr id="10" name="Chart 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -14283,7 +14431,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -14313,7 +14467,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="12" name="Chart 11"/>
+        <xdr:cNvPr id="12" name="Chart 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -14343,7 +14503,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -14373,7 +14539,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -14653,31 +14825,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M72"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="S72" sqref="S72"/>
+      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="6.84375" customWidth="1"/>
+    <col min="2" max="2" width="8.84375" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" customWidth="1"/>
+    <col min="4" max="4" width="7.3828125" customWidth="1"/>
+    <col min="5" max="5" width="6.53515625" customWidth="1"/>
+    <col min="6" max="6" width="8.15234375" customWidth="1"/>
+    <col min="7" max="7" width="11.53515625" customWidth="1"/>
+    <col min="8" max="8" width="7.3828125" customWidth="1"/>
+    <col min="9" max="9" width="7.3046875" customWidth="1"/>
+    <col min="10" max="10" width="7.53515625" customWidth="1"/>
+    <col min="11" max="11" width="7.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14714,8 +14886,11 @@
       <c r="M1" s="6" t="s">
         <v>71</v>
       </c>
+      <c r="N1" s="6" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -14753,8 +14928,12 @@
         <f>(SQRT((I2*J2)/3.1415927))*2</f>
         <v>3.4869545139576457</v>
       </c>
+      <c r="N2">
+        <f>M2*25.4</f>
+        <v>88.568644654524192</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -14792,8 +14971,12 @@
         <f t="shared" ref="M3:M59" si="0">(SQRT((I3*J3)/3.1415927))*2</f>
         <v>3.3552479039060641</v>
       </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N59" si="1">M3*25.4</f>
+        <v>85.223296759214023</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -14831,8 +15014,12 @@
         <f t="shared" si="0"/>
         <v>3.2285875739527143</v>
       </c>
+      <c r="N4">
+        <f t="shared" si="1"/>
+        <v>82.006124378398937</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -14870,8 +15057,12 @@
         <f t="shared" si="0"/>
         <v>3.1063409298704627</v>
       </c>
+      <c r="N5">
+        <f t="shared" si="1"/>
+        <v>78.901059618709752</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -14909,8 +15100,12 @@
         <f t="shared" si="0"/>
         <v>2.9892699860158531</v>
       </c>
+      <c r="N6">
+        <f t="shared" si="1"/>
+        <v>75.927457644802672</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -14948,8 +15143,12 @@
         <f t="shared" si="0"/>
         <v>2.8759801630858233</v>
       </c>
+      <c r="N7">
+        <f t="shared" si="1"/>
+        <v>73.049896142379907</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -14987,8 +15186,12 @@
         <f t="shared" si="0"/>
         <v>2.7672334232585678</v>
       </c>
+      <c r="N8">
+        <f t="shared" si="1"/>
+        <v>70.287728950767615</v>
+      </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -15026,8 +15229,12 @@
         <f t="shared" si="0"/>
         <v>2.6630297986855833</v>
       </c>
+      <c r="N9">
+        <f t="shared" si="1"/>
+        <v>67.640956886613807</v>
+      </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -15065,8 +15272,12 @@
         <f t="shared" si="0"/>
         <v>2.56210408879878</v>
       </c>
+      <c r="N10">
+        <f t="shared" si="1"/>
+        <v>65.077443855489008</v>
+      </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -15104,8 +15315,12 @@
         <f t="shared" si="0"/>
         <v>2.4657214762158479</v>
       </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>62.629325495882533</v>
+      </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -15143,8 +15358,12 @@
         <f t="shared" si="0"/>
         <v>2.3726167524485509</v>
       </c>
+      <c r="N12">
+        <f t="shared" si="1"/>
+        <v>60.26446551219319</v>
+      </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -15182,8 +15401,12 @@
         <f t="shared" si="0"/>
         <v>2.2829193576917066</v>
       </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>57.986151685369343</v>
+      </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -15221,8 +15444,12 @@
         <f t="shared" si="0"/>
         <v>2.1966293616645363</v>
       </c>
+      <c r="N14">
+        <f t="shared" si="1"/>
+        <v>55.794385786279221</v>
+      </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -15260,8 +15487,12 @@
         <f t="shared" si="0"/>
         <v>2.1137466310857307</v>
       </c>
+      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>53.689164429577559</v>
+      </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -15299,8 +15530,12 @@
         <f t="shared" si="0"/>
         <v>2.0335092452720707</v>
       </c>
+      <c r="N16">
+        <f t="shared" si="1"/>
+        <v>51.651134829910589</v>
+      </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
@@ -15338,8 +15573,12 @@
         <f t="shared" si="0"/>
         <v>1.9573118065732584</v>
       </c>
+      <c r="N17">
+        <f t="shared" si="1"/>
+        <v>49.715719886960763</v>
+      </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -15377,8 +15616,12 @@
         <f t="shared" si="0"/>
         <v>1.8827532912399096</v>
       </c>
+      <c r="N18">
+        <f t="shared" si="1"/>
+        <v>47.821933597493704</v>
+      </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -15416,8 +15659,12 @@
         <f t="shared" si="0"/>
         <v>1.8121052621267633</v>
       </c>
+      <c r="N19">
+        <f t="shared" si="1"/>
+        <v>46.027473658019787</v>
+      </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -15455,8 +15702,12 @@
         <f t="shared" si="0"/>
         <v>1.7437288228494028</v>
       </c>
+      <c r="N20">
+        <f t="shared" si="1"/>
+        <v>44.290712100374826</v>
+      </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -15494,8 +15745,12 @@
         <f t="shared" si="0"/>
         <v>1.677623951953032</v>
       </c>
+      <c r="N21">
+        <f t="shared" si="1"/>
+        <v>42.611648379607011</v>
+      </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
@@ -15533,8 +15788,12 @@
         <f t="shared" si="0"/>
         <v>1.6142937869763572</v>
       </c>
+      <c r="N22">
+        <f t="shared" si="1"/>
+        <v>41.003062189199468</v>
+      </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -15572,8 +15831,12 @@
         <f t="shared" si="0"/>
         <v>1.5532351227944652</v>
       </c>
+      <c r="N23">
+        <f t="shared" si="1"/>
+        <v>39.452172118979412</v>
+      </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
@@ -15611,8 +15874,12 @@
         <f t="shared" si="0"/>
         <v>1.4943187016081292</v>
       </c>
+      <c r="N24">
+        <f t="shared" si="1"/>
+        <v>37.955695020846477</v>
+      </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -15650,8 +15917,12 @@
         <f t="shared" si="0"/>
         <v>1.4383063666191094</v>
       </c>
+      <c r="N25">
+        <f t="shared" si="1"/>
+        <v>36.532981712125377</v>
+      </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
@@ -15692,8 +15963,12 @@
         <f t="shared" si="0"/>
         <v>1.3839330030293759</v>
       </c>
+      <c r="N26">
+        <f t="shared" si="1"/>
+        <v>35.151898276946149</v>
+      </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>36</v>
       </c>
@@ -15734,8 +16009,12 @@
         <f t="shared" si="0"/>
         <v>1.3311985874487118</v>
       </c>
+      <c r="N27">
+        <f t="shared" si="1"/>
+        <v>33.812444121197281</v>
+      </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
@@ -15776,8 +16055,12 @@
         <f t="shared" si="0"/>
         <v>1.2813683145052823</v>
       </c>
+      <c r="N28">
+        <f t="shared" si="1"/>
+        <v>32.546755188434169</v>
+      </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>38</v>
       </c>
@@ -15818,8 +16101,12 @@
         <f t="shared" si="0"/>
         <v>1.2325444171949285</v>
       </c>
+      <c r="N29">
+        <f t="shared" si="1"/>
+        <v>31.306628196751181</v>
+      </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
@@ -15860,8 +16147,12 @@
         <f t="shared" si="0"/>
         <v>1.1866246829559928</v>
       </c>
+      <c r="N30">
+        <f t="shared" si="1"/>
+        <v>30.140266947082214</v>
+      </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
@@ -15902,8 +16193,12 @@
         <f t="shared" si="0"/>
         <v>1.1412081174810693</v>
       </c>
+      <c r="N31">
+        <f t="shared" si="1"/>
+        <v>28.98668618401916</v>
+      </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
@@ -15944,8 +16239,12 @@
         <f t="shared" si="0"/>
         <v>1.0980630911643625</v>
       </c>
+      <c r="N32">
+        <f t="shared" si="1"/>
+        <v>27.890802515574805</v>
+      </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
@@ -15986,8 +16285,12 @@
         <f t="shared" si="0"/>
         <v>1.0565570284444934</v>
       </c>
+      <c r="N33">
+        <f t="shared" si="1"/>
+        <v>26.83654852249013</v>
+      </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
         <v>43</v>
       </c>
@@ -16028,8 +16331,12 @@
         <f t="shared" si="0"/>
         <v>1.0173225197603968</v>
       </c>
+      <c r="N34">
+        <f t="shared" si="1"/>
+        <v>25.839992001914077</v>
+      </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
         <v>44</v>
       </c>
@@ -16070,8 +16377,12 @@
         <f t="shared" si="0"/>
         <v>0.97808801098956144</v>
       </c>
+      <c r="N35">
+        <f t="shared" si="1"/>
+        <v>24.843435479134858</v>
+      </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>45</v>
       </c>
@@ -16112,8 +16423,12 @@
         <f t="shared" si="0"/>
         <v>0.941628182470301</v>
       </c>
+      <c r="N36">
+        <f t="shared" si="1"/>
+        <v>23.917355834745646</v>
+      </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
         <v>46</v>
       </c>
@@ -16154,8 +16469,12 @@
         <f t="shared" si="0"/>
         <v>0.90580105459565174</v>
       </c>
+      <c r="N37">
+        <f t="shared" si="1"/>
+        <v>23.007346786729553</v>
+      </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
         <v>47</v>
       </c>
@@ -16196,8 +16515,12 @@
         <f t="shared" si="0"/>
         <v>0.87161282740231605</v>
       </c>
+      <c r="N38">
+        <f t="shared" si="1"/>
+        <v>22.138965816018825</v>
+      </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
         <v>48</v>
       </c>
@@ -16238,8 +16561,12 @@
         <f t="shared" si="0"/>
         <v>0.83906353153052238</v>
       </c>
+      <c r="N39">
+        <f t="shared" si="1"/>
+        <v>21.312213700875269</v>
+      </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
         <v>49</v>
       </c>
@@ -16280,8 +16607,12 @@
         <f t="shared" si="0"/>
         <v>0.80714689348817859</v>
       </c>
+      <c r="N40">
+        <f t="shared" si="1"/>
+        <v>20.501531094599734</v>
+      </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
         <v>50</v>
       </c>
@@ -16322,8 +16653,12 @@
         <f t="shared" si="0"/>
         <v>0.77686917895167107</v>
       </c>
+      <c r="N41">
+        <f t="shared" si="1"/>
+        <v>19.732477145372442</v>
+      </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
         <v>51</v>
       </c>
@@ -16364,8 +16699,12 @@
         <f t="shared" si="0"/>
         <v>0.74772724167831561</v>
       </c>
+      <c r="N42">
+        <f t="shared" si="1"/>
+        <v>18.992271938629216</v>
+      </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A43" s="2">
         <v>2</v>
       </c>
@@ -16406,8 +16745,12 @@
         <f t="shared" si="0"/>
         <v>0.71908833690235296</v>
       </c>
+      <c r="N43">
+        <f t="shared" si="1"/>
+        <v>18.264843757319763</v>
+      </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
         <v>52</v>
       </c>
@@ -16448,8 +16791,12 @@
         <f t="shared" si="0"/>
         <v>0.69221807996383433</v>
       </c>
+      <c r="N44">
+        <f t="shared" si="1"/>
+        <v>17.582339231081392</v>
+      </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
         <v>53</v>
       </c>
@@ -16490,8 +16837,12 @@
         <f t="shared" si="0"/>
         <v>0.66585079545021186</v>
       </c>
+      <c r="N45">
+        <f t="shared" si="1"/>
+        <v>16.912610204435381</v>
+      </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
         <v>54</v>
       </c>
@@ -16532,8 +16883,12 @@
         <f t="shared" si="0"/>
         <v>0.64061931790686777</v>
       </c>
+      <c r="N46">
+        <f t="shared" si="1"/>
+        <v>16.271730674834441</v>
+      </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
         <v>55</v>
       </c>
@@ -16574,8 +16929,12 @@
         <f t="shared" si="0"/>
         <v>0.61652369696075704</v>
       </c>
+      <c r="N47">
+        <f t="shared" si="1"/>
+        <v>15.659701902803228</v>
+      </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
         <v>56</v>
       </c>
@@ -16616,8 +16975,12 @@
         <f t="shared" si="0"/>
         <v>0.59306067133243034</v>
       </c>
+      <c r="N48">
+        <f t="shared" si="1"/>
+        <v>15.06374105184373</v>
+      </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
         <v>57</v>
       </c>
@@ -16658,8 +17021,12 @@
         <f t="shared" si="0"/>
         <v>0.57060405874053466</v>
       </c>
+      <c r="N49">
+        <f t="shared" si="1"/>
+        <v>14.49334309200958</v>
+      </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
         <v>58</v>
       </c>
@@ -16700,8 +17067,12 @@
         <f t="shared" si="0"/>
         <v>0.54928310644100897</v>
       </c>
+      <c r="N50">
+        <f t="shared" si="1"/>
+        <v>13.951790903601626</v>
+      </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
         <v>59</v>
       </c>
@@ -16742,8 +17113,12 @@
         <f t="shared" si="0"/>
         <v>0.52859475400766132</v>
       </c>
+      <c r="N51">
+        <f t="shared" si="1"/>
+        <v>13.426306751794597</v>
+      </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
         <v>60</v>
       </c>
@@ -16784,8 +17159,12 @@
         <f t="shared" si="0"/>
         <v>0.50840963421064278</v>
       </c>
+      <c r="N52">
+        <f t="shared" si="1"/>
+        <v>12.913604708950325</v>
+      </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A53" s="1" t="s">
         <v>61</v>
       </c>
@@ -16826,8 +17205,12 @@
         <f t="shared" si="0"/>
         <v>0.48936023184886929</v>
       </c>
+      <c r="N53">
+        <f t="shared" si="1"/>
+        <v>12.429749888961279</v>
+      </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A54" s="1" t="s">
         <v>62</v>
       </c>
@@ -16868,8 +17251,12 @@
         <f t="shared" si="0"/>
         <v>0.4708140912351505</v>
       </c>
+      <c r="N54">
+        <f t="shared" si="1"/>
+        <v>11.958677917372823</v>
+      </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A55" s="2">
         <v>3</v>
       </c>
@@ -16910,8 +17297,12 @@
         <f t="shared" si="0"/>
         <v>0.45290052729782587</v>
       </c>
+      <c r="N55">
+        <f t="shared" si="1"/>
+        <v>11.503673393364776</v>
+      </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A56" s="1" t="s">
         <v>63</v>
       </c>
@@ -16952,8 +17343,12 @@
         <f t="shared" si="0"/>
         <v>0.43612255912808251</v>
       </c>
+      <c r="N56">
+        <f t="shared" si="1"/>
+        <v>11.077513001853296</v>
+      </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A57" s="1" t="s">
         <v>64</v>
       </c>
@@ -16994,8 +17389,12 @@
         <f t="shared" si="0"/>
         <v>0.41921525740955856</v>
       </c>
+      <c r="N57">
+        <f t="shared" si="1"/>
+        <v>10.648067538202787</v>
+      </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
@@ -17036,8 +17435,12 @@
         <f t="shared" si="0"/>
         <v>0.40357344674408929</v>
       </c>
+      <c r="N58">
+        <f t="shared" si="1"/>
+        <v>10.250765547299867</v>
+      </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A59" s="1" t="s">
         <v>66</v>
       </c>
@@ -17078,8 +17481,12 @@
         <f t="shared" si="0"/>
         <v>0.38843458947583553</v>
       </c>
+      <c r="N59">
+        <f t="shared" si="1"/>
+        <v>9.8662385726862212</v>
+      </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="B60" s="1" t="s">
         <v>1</v>
       </c>
@@ -17111,12 +17518,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A64" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A65" s="1" t="s">
         <v>1</v>
       </c>
@@ -17148,7 +17555,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>2093</v>
       </c>
@@ -17191,58 +17598,58 @@
         <v>69</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B67">
         <f>B66*25.4</f>
         <v>2.8257920284355804</v>
       </c>
       <c r="C67">
-        <f t="shared" ref="C67:F67" si="1">C66*25.4</f>
+        <f t="shared" ref="C67:F67" si="2">C66*25.4</f>
         <v>24.500354340087945</v>
       </c>
       <c r="D67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19.049999999999997</v>
       </c>
       <c r="E67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.50689392885142859</v>
       </c>
       <c r="F67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9102758865308371</v>
       </c>
       <c r="G67" t="s">
         <v>68</v>
       </c>
       <c r="H67">
-        <f t="shared" ref="H67" si="2">H66*25.4</f>
+        <f t="shared" ref="H67" si="3">H66*25.4</f>
         <v>6.9262626689507174</v>
       </c>
       <c r="I67">
-        <f t="shared" ref="I67" si="3">I66*25.4</f>
+        <f t="shared" ref="I67" si="4">I66*25.4</f>
         <v>8.707067170327857</v>
       </c>
       <c r="J67">
-        <f t="shared" ref="J67" si="4">J66*25.4</f>
+        <f t="shared" ref="J67" si="5">J66*25.4</f>
         <v>30.337677937540398</v>
       </c>
       <c r="K67" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.4">
       <c r="G68">
         <v>0.25</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.4">
       <c r="G69">
         <f>0.25*25.4</f>
         <v>6.35</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.4">
       <c r="E72">
         <f>1046.5*2</f>
         <v>2093</v>

</xml_diff>